<commit_message>
updated the mtbenv to use the correct manifest, depending on the settings include lcs
</commit_message>
<xml_diff>
--- a/extension/docs/testcases.xlsx
+++ b/extension/docs/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\src\mtbassist\extension\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5479410D-5A4F-4A9D-9AB3-2BA9D4C18E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC17304-751E-4122-AB0F-348D77EED416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{0C2101DC-B55E-4BC5-A376-ECF5E5FC8A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Test No</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>If LCS is enabled, read manifest files from LCS</t>
+  </si>
+  <si>
+    <t>Various combinations of closing the window and re-opening</t>
+  </si>
+  <si>
+    <t>Interaction with LCS manager and EAP</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F388CE65-71E5-4E4F-8CE5-B45C2E9937B5}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -474,6 +480,22 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>